<commit_message>
added Login Home and Graph code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AEEDA09C-166B-4360-BF8F-C2EED295055F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\BDDAlgo\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E664C9B-3C7B-4BB7-BFB7-94A0832D7432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39825" yWindow="885" windowWidth="14400" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -57,13 +61,37 @@
   </si>
   <si>
     <t>welc</t>
+  </si>
+  <si>
+    <t>Drop-down</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Graph</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +105,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,9 +137,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
@@ -413,19 +445,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -441,7 +473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -449,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -457,53 +489,109 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -513,6 +601,8 @@
     <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{7004777B-9E3D-4F5C-8944-3CB8C78DB409}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{FE4F4546-DDBE-4951-BA0A-778E6DEBC0EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -522,9 +612,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -536,7 +631,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tree files with updated excel data file and updated excelreader class file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\BDDAlgo\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E664C9B-3C7B-4BB7-BFB7-94A0832D7432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39825" yWindow="885" windowWidth="14400" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="tryeditor" sheetId="2" r:id="rId2"/>
+    <sheet name="practiceq" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -54,44 +48,108 @@
     <t>Jewel Space</t>
   </si>
   <si>
+    <t>welc</t>
+  </si>
+  <si>
     <t>Jeweluser</t>
   </si>
   <si>
     <t>Jeweluser1</t>
   </si>
   <si>
-    <t>welc</t>
-  </si>
-  <si>
-    <t>Drop-down</t>
-  </si>
-  <si>
-    <t>Data Structures</t>
-  </si>
-  <si>
-    <t>Arrays</t>
-  </si>
-  <si>
-    <t>Linked List</t>
-  </si>
-  <si>
-    <t>Stack</t>
-  </si>
-  <si>
-    <t>Queue</t>
-  </si>
-  <si>
-    <t>Tree</t>
-  </si>
-  <si>
-    <t>Graph</t>
+    <t>Code to use in try editor</t>
+  </si>
+  <si>
+    <t>Invalid code</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>print("hello")</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>PracticeQuestion</t>
+  </si>
+  <si>
+    <t>Run Output</t>
+  </si>
+  <si>
+    <t>Submit output</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+  if(num in input_list):
+    print("Element Found")
+  else:
+    print("Not Found")
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0
+    return max_count
+nums = [1, 1, 0, 1, 1, 1]
+print(findMaxConsecutiveOnes(nums))</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+nums = [54521, 25, 46, 17896]
+print(findNumbers(nums))</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    result = []
+    left, right = 0, len(nums) - 1
+    while left &lt;= right:
+        if abs(nums[left]) &gt; abs(nums[right]):
+            result.append(nums[left] ** 2)
+            left += 1
+        else:
+            result.append(nums[right] ** 2)
+            right -= 1
+    return result[::-1]
+nums = [-4, -1, 0, 3, 10]
+print(sortedSquares(nums))</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):~
+max_count = 0
+@current_count = 0
+for num in nums:
+if num == 1:
+current_count += 1
+max_count = max(max_count, current_count)
+else:
+current_count = 0
+return max_count
+nums = [1, 1, 0, 1, 1, 1]
+print(findMaxConsecutiveOnes(nums))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,21 +165,40 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,21 +206,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -159,9 +265,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +305,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -233,7 +339,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -268,10 +373,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -444,20 +548,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -473,7 +578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -481,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -489,12 +594,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -502,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -510,23 +615,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -534,105 +639,118 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{7EAA162E-3D46-4B3A-BB4C-20DD4B95624B}"/>
-    <hyperlink ref="A7" r:id="rId4" display="Jewel@" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B12" r:id="rId9" xr:uid="{7004777B-9E3D-4F5C-8944-3CB8C78DB409}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{FE4F4546-DDBE-4951-BA0A-778E6DEBC0EA}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4" display="Jewel@"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="86.4">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="172.8">
+      <c r="A3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="115.2">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="187.2">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="172.8">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add row in excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\TestBDD\MavericksBDD\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D3C2FC-3855-4E16-8C83-2FC77E45ED0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -144,11 +150,35 @@
 nums = [1, 1, 0, 1, 1, 1]
 print(findMaxConsecutiveOnes(nums))</t>
   </si>
+  <si>
+    <t>Drop-down</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -249,7 +279,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,9 +295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +335,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -339,6 +369,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -373,9 +404,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,18 +580,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -639,30 +671,76 @@
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="A7" r:id="rId4" display="Jewel@"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
@@ -676,7 +754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -698,17 +776,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -722,27 +800,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="86.4">
+    <row r="2" spans="1:3" ht="87">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="172.8">
+    <row r="3" spans="1:3" ht="174">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="115.2">
+    <row r="4" spans="1:3" ht="116">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="187.2">
+    <row r="5" spans="1:3" ht="188.5">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="172.8">
+    <row r="6" spans="1:3" ht="174">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Adding Array and Data structure files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\TestBDD\MavericksBDD\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D3C2FC-3855-4E16-8C83-2FC77E45ED0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>username</t>
   </si>
@@ -84,73 +78,6 @@
     <t>PracticeQuestion</t>
   </si>
   <si>
-    <t>Run Output</t>
-  </si>
-  <si>
-    <t>Submit output</t>
-  </si>
-  <si>
-    <t>def search(input_list, num):
-  if(num in input_list):
-    print("Element Found")
-  else:
-    print("Not Found")
-search([12, 23, 45, 67, 6, 90] , 12)</t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums):
-    max_count = 0
-    current_count = 0
-    for num in nums:
-        if num == 1:
-            current_count += 1
-            max_count = max(max_count, current_count)
-        else:
-            current_count = 0
-    return max_count
-nums = [1, 1, 0, 1, 1, 1]
-print(findMaxConsecutiveOnes(nums))</t>
-  </si>
-  <si>
-    <t>def findNumbers(nums):
-    count = 0
-    for num in nums:
-        if len(str(num)) % 2 == 0:
-            count += 1
-    return count
-nums = [54521, 25, 46, 17896]
-print(findNumbers(nums))</t>
-  </si>
-  <si>
-    <t>def sortedSquares(nums):
-    result = []
-    left, right = 0, len(nums) - 1
-    while left &lt;= right:
-        if abs(nums[left]) &gt; abs(nums[right]):
-            result.append(nums[left] ** 2)
-            left += 1
-        else:
-            result.append(nums[right] ** 2)
-            right -= 1
-    return result[::-1]
-nums = [-4, -1, 0, 3, 10]
-print(sortedSquares(nums))</t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums):~
-max_count = 0
-@current_count = 0
-for num in nums:
-if num == 1:
-current_count += 1
-max_count = max(max_count, current_count)
-else:
-current_count = 0
-return max_count
-nums = [1, 1, 0, 1, 1, 1]
-print(findMaxConsecutiveOnes(nums))</t>
-  </si>
-  <si>
     <t>Drop-down</t>
   </si>
   <si>
@@ -173,13 +100,29 @@
   </si>
   <si>
     <t>Graph</t>
+  </si>
+  <si>
+    <t>@def search(input_list, num):~if(num in input_list): ~print("Element Found")~@@else:~print("Not Found")~@@@@search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>@def findMaxConsecutiveOnes(nums):~max_count = 0~current_count = 0~for num in nums:~  if num == 1:~         @@@@@@@current_count += 1~max_count = max(max_count, current_count)~@@@@else:~   @current_count = 0~@@@@@@@@return max_count~nums = [1, 1, 0, 1, 1, 1]~print(findMaxConsecutiveOnes(nums))</t>
+  </si>
+  <si>
+    <t>@def findNumbers(nums):~  count = 0~  @@for num in nums:~  if len(str(num)) % 2 == 0:~         @@@@@@@count += 1~@@@@@@@@return count~@@nums = [54521, 25, 46, 17896]~ @print(findNumbers(nums))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@def sortedSquares(nums):~  result = []~  @@left, right = 0, len(nums) - 1~  @@while left &lt;= right:~  if abs(nums[left]) &gt; abs(nums[right]):~         @@@@@@@result.append(nums[left] ** 2)~         @@@@@@@@@left += 1~   @@@@@@@else:~   @result.append(nums[right] ** 2)~   @@@right -= 1~  @@@@@@@@@@return result[::-1]~@@nums = [-4, -1, 0, 3, 10]~ @print(sortedSquares(nums))
+</t>
+  </si>
+  <si>
+    <t>Second last try</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +155,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -266,20 +214,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -295,9 +243,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -335,7 +283,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -369,7 +317,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -404,10 +351,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -580,18 +526,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.90625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -689,42 +635,42 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -733,14 +679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
@@ -754,7 +700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -776,57 +722,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="106.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="207.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="87">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="174">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="116">
-      <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="188.5">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="174">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5"/>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="28.8">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="43.2">
+      <c r="A5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>